<commit_message>
updated mapping file and refactored code
</commit_message>
<xml_diff>
--- a/src/main/resources/EmployeeMapping.xlsx
+++ b/src/main/resources/EmployeeMapping.xlsx
@@ -776,7 +776,7 @@
     <t>FWIN02010</t>
   </si>
   <si>
-    <t>E88399</t>
+    <t>E088399</t>
   </si>
   <si>
     <t>Kunal Jadhav</t>
@@ -1028,7 +1028,7 @@
     <t>Charan Rathi</t>
   </si>
   <si>
-    <t>FJ256</t>
+    <t>FL256</t>
   </si>
   <si>
     <t>E109858</t>
@@ -1742,7 +1742,7 @@
     <t>Vikram Giriraj</t>
   </si>
   <si>
-    <t>FD00549</t>
+    <t>FDIED0011</t>
   </si>
   <si>
     <t>E171734</t>
@@ -2163,7 +2163,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2173,13 +2173,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2667,28 +2660,31 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2697,118 +2693,115 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3157,7 +3150,7 @@
   <dimension ref="A1:D249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -5048,7 +5041,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="137" ht="28.8" spans="1:4">
+    <row r="137" spans="1:4">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -6574,7 +6567,7 @@
     </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:D249" etc:filterBottomFollowUsedRange="0">
-    <sortState ref="A2:D249">
+    <sortState ref="A1:D249">
       <sortCondition ref="A1"/>
     </sortState>
     <extLst/>

</xml_diff>